<commit_message>
This is the commit for TestData.xlsx file
</commit_message>
<xml_diff>
--- a/HybridFramework_Demo/src/test/resources/testData/TestData.xlsx
+++ b/HybridFramework_Demo/src/test/resources/testData/TestData.xlsx
@@ -24,31 +24,31 @@
     <t>Product Type</t>
   </si>
   <si>
-    <t>Product Number</t>
-  </si>
-  <si>
-    <t>First Name</t>
-  </si>
-  <si>
-    <t>Last Name</t>
+    <t>Product Sub Type</t>
+  </si>
+  <si>
+    <t>Min Budget</t>
+  </si>
+  <si>
+    <t>Max Budget</t>
   </si>
   <si>
     <t>Address</t>
   </si>
   <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>Phone</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Result</t>
+    <t>Min Bedroom</t>
+  </si>
+  <si>
+    <t>Max Bedroom</t>
+  </si>
+  <si>
+    <t>Home Price</t>
+  </si>
+  <si>
+    <t>Down Payment</t>
+  </si>
+  <si>
+    <t>Mortgage Interest Rate</t>
   </si>
   <si>
     <t>Framework_001</t>
@@ -57,7 +57,7 @@
     <t>Mozilla</t>
   </si>
   <si>
-    <t>Accessories</t>
+    <t>Buy</t>
   </si>
   <si>
     <t>Product 2</t>
@@ -95,7 +95,7 @@
     <t>Framework_002</t>
   </si>
   <si>
-    <t>iMacs</t>
+    <t>Mortgage</t>
   </si>
   <si>
     <t>Product 1</t>
@@ -114,7 +114,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -126,17 +126,22 @@
       <name val="Helvetica"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color indexed="8"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <b val="1"/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="1"/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
@@ -162,7 +167,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -260,6 +265,17 @@
       <left style="thin">
         <color indexed="10"/>
       </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -303,6 +319,19 @@
       <right style="thin">
         <color indexed="10"/>
       </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
       <top style="thin">
         <color indexed="10"/>
       </top>
@@ -317,12 +346,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
@@ -330,47 +359,59 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="5" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="5" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="5" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="5" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="5" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="5" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="5" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="5" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
+    <xf numFmtId="1" fontId="5" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1620,7 +1661,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1633,12 +1674,13 @@
     <col min="5" max="5" width="7.875" style="1" customWidth="1"/>
     <col min="6" max="6" width="7.625" style="1" customWidth="1"/>
     <col min="7" max="7" width="13.125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="7.75" style="1" customWidth="1"/>
-    <col min="9" max="9" width="18.75" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.25" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5" style="1" customWidth="1"/>
     <col min="10" max="10" width="8.25" style="1" customWidth="1"/>
     <col min="11" max="11" width="15" style="1" customWidth="1"/>
-    <col min="12" max="12" width="6.625" style="1" customWidth="1"/>
-    <col min="13" max="256" width="6.625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="15.25" style="1" customWidth="1"/>
+    <col min="13" max="13" width="6.625" style="1" customWidth="1"/>
+    <col min="14" max="256" width="6.625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="30" customHeight="1">
@@ -1678,181 +1720,229 @@
       <c r="L1" t="s" s="3">
         <v>11</v>
       </c>
+      <c r="M1" s="4"/>
     </row>
     <row r="2" ht="17" customHeight="1">
-      <c r="A2" t="s" s="4">
+      <c r="A2" t="s" s="5">
         <v>12</v>
       </c>
-      <c r="B2" t="s" s="4">
+      <c r="B2" t="s" s="5">
         <v>13</v>
       </c>
-      <c r="C2" t="s" s="4">
+      <c r="C2" t="s" s="5">
         <v>14</v>
       </c>
-      <c r="D2" t="s" s="4">
+      <c r="D2" t="s" s="5">
         <v>15</v>
       </c>
-      <c r="E2" t="s" s="4">
+      <c r="E2" t="s" s="5">
         <v>16</v>
       </c>
-      <c r="F2" t="s" s="4">
+      <c r="F2" t="s" s="5">
         <v>17</v>
       </c>
-      <c r="G2" t="s" s="4">
+      <c r="G2" t="s" s="5">
         <v>18</v>
       </c>
-      <c r="H2" t="s" s="4">
+      <c r="H2" t="s" s="5">
         <v>19</v>
       </c>
-      <c r="I2" t="s" s="4">
+      <c r="I2" t="s" s="5">
         <v>20</v>
       </c>
-      <c r="J2" t="s" s="4">
+      <c r="J2" t="s" s="5">
         <v>21</v>
       </c>
-      <c r="K2" t="s" s="5">
+      <c r="K2" t="s" s="6">
         <v>22</v>
       </c>
-      <c r="L2" s="6"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="8"/>
     </row>
     <row r="3" ht="17" customHeight="1">
-      <c r="A3" t="s" s="4">
+      <c r="A3" t="s" s="5">
         <v>23</v>
       </c>
-      <c r="B3" t="s" s="4">
+      <c r="B3" t="s" s="5">
         <v>13</v>
       </c>
-      <c r="C3" t="s" s="4">
+      <c r="C3" t="s" s="5">
         <v>24</v>
       </c>
-      <c r="D3" t="s" s="4">
+      <c r="D3" t="s" s="5">
         <v>25</v>
       </c>
-      <c r="E3" t="s" s="4">
+      <c r="E3" t="s" s="5">
         <v>26</v>
       </c>
-      <c r="F3" t="s" s="4">
+      <c r="F3" t="s" s="5">
         <v>17</v>
       </c>
-      <c r="G3" t="s" s="4">
+      <c r="G3" t="s" s="5">
         <v>27</v>
       </c>
-      <c r="H3" t="s" s="4">
+      <c r="H3" t="s" s="5">
         <v>19</v>
       </c>
-      <c r="I3" t="s" s="4">
+      <c r="I3" t="s" s="5">
         <v>20</v>
       </c>
-      <c r="J3" t="s" s="4">
+      <c r="J3" t="s" s="5">
         <v>21</v>
       </c>
-      <c r="K3" t="s" s="5">
+      <c r="K3" t="s" s="6">
         <v>22</v>
       </c>
-      <c r="L3" s="6"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="8"/>
     </row>
     <row r="4" ht="17" customHeight="1">
-      <c r="A4" s="7"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="10"/>
+      <c r="A4" t="s" s="5">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s" s="5">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s" s="5">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s" s="5">
+        <v>25</v>
+      </c>
+      <c r="E4" t="s" s="5">
+        <v>26</v>
+      </c>
+      <c r="F4" t="s" s="5">
+        <v>17</v>
+      </c>
+      <c r="G4" t="s" s="5">
+        <v>27</v>
+      </c>
+      <c r="H4" t="s" s="5">
+        <v>19</v>
+      </c>
+      <c r="I4" t="s" s="5">
+        <v>20</v>
+      </c>
+      <c r="J4" t="s" s="5">
+        <v>21</v>
+      </c>
+      <c r="K4" t="s" s="6">
+        <v>22</v>
+      </c>
+      <c r="L4" s="7"/>
+      <c r="M4" s="8"/>
     </row>
     <row r="5" ht="17" customHeight="1">
-      <c r="A5" s="11"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="10"/>
+      <c r="A5" s="9"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="13"/>
     </row>
     <row r="6" ht="17" customHeight="1">
-      <c r="A6" s="11"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="10"/>
+      <c r="A6" s="14"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="13"/>
     </row>
     <row r="7" ht="17" customHeight="1">
-      <c r="A7" s="11"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="10"/>
+      <c r="A7" s="14"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="13"/>
     </row>
     <row r="8" ht="17" customHeight="1">
-      <c r="A8" s="11"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="10"/>
+      <c r="A8" s="14"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="13"/>
     </row>
     <row r="9" ht="17" customHeight="1">
-      <c r="A9" s="11"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="10"/>
+      <c r="A9" s="14"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="13"/>
     </row>
     <row r="10" ht="17" customHeight="1">
-      <c r="A10" s="12"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="14"/>
+      <c r="A10" s="14"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="13"/>
+    </row>
+    <row r="11" ht="17" customHeight="1">
+      <c r="A11" s="15"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="18"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="K2" r:id="rId1" location="" tooltip="" display=""/>
     <hyperlink ref="K3" r:id="rId2" location="" tooltip="" display=""/>
+    <hyperlink ref="K4" r:id="rId3" location="" tooltip="" display=""/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
@@ -1870,83 +1960,83 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.625" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="6.625" style="15" customWidth="1"/>
-    <col min="2" max="2" width="6.625" style="15" customWidth="1"/>
-    <col min="3" max="3" width="6.625" style="15" customWidth="1"/>
-    <col min="4" max="4" width="6.625" style="15" customWidth="1"/>
-    <col min="5" max="5" width="6.625" style="15" customWidth="1"/>
-    <col min="6" max="256" width="6.625" style="15" customWidth="1"/>
+    <col min="1" max="1" width="6.625" style="19" customWidth="1"/>
+    <col min="2" max="2" width="6.625" style="19" customWidth="1"/>
+    <col min="3" max="3" width="6.625" style="19" customWidth="1"/>
+    <col min="4" max="4" width="6.625" style="19" customWidth="1"/>
+    <col min="5" max="5" width="6.625" style="19" customWidth="1"/>
+    <col min="6" max="256" width="6.625" style="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="17" customHeight="1">
-      <c r="A1" s="16"/>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
+      <c r="A1" s="20"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
     </row>
     <row r="2" ht="17" customHeight="1">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
     </row>
     <row r="3" ht="17" customHeight="1">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
+      <c r="A3" s="20"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
     </row>
     <row r="4" ht="17" customHeight="1">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
+      <c r="A4" s="20"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
     </row>
     <row r="5" ht="17" customHeight="1">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
+      <c r="A5" s="20"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
     </row>
     <row r="6" ht="17" customHeight="1">
-      <c r="A6" s="16"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
+      <c r="A6" s="20"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
     </row>
     <row r="7" ht="17" customHeight="1">
-      <c r="A7" s="16"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
+      <c r="A7" s="20"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
     </row>
     <row r="8" ht="17" customHeight="1">
-      <c r="A8" s="16"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
+      <c r="A8" s="20"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
     </row>
     <row r="9" ht="17" customHeight="1">
-      <c r="A9" s="16"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
+      <c r="A9" s="20"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
     </row>
     <row r="10" ht="17" customHeight="1">
-      <c r="A10" s="16"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
+      <c r="A10" s="20"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1965,83 +2055,83 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.625" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="6.625" style="17" customWidth="1"/>
-    <col min="2" max="2" width="6.625" style="17" customWidth="1"/>
-    <col min="3" max="3" width="6.625" style="17" customWidth="1"/>
-    <col min="4" max="4" width="6.625" style="17" customWidth="1"/>
-    <col min="5" max="5" width="6.625" style="17" customWidth="1"/>
-    <col min="6" max="256" width="6.625" style="17" customWidth="1"/>
+    <col min="1" max="1" width="6.625" style="21" customWidth="1"/>
+    <col min="2" max="2" width="6.625" style="21" customWidth="1"/>
+    <col min="3" max="3" width="6.625" style="21" customWidth="1"/>
+    <col min="4" max="4" width="6.625" style="21" customWidth="1"/>
+    <col min="5" max="5" width="6.625" style="21" customWidth="1"/>
+    <col min="6" max="256" width="6.625" style="21" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="17" customHeight="1">
-      <c r="A1" s="16"/>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
+      <c r="A1" s="20"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
     </row>
     <row r="2" ht="17" customHeight="1">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
     </row>
     <row r="3" ht="17" customHeight="1">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
+      <c r="A3" s="20"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
     </row>
     <row r="4" ht="17" customHeight="1">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
+      <c r="A4" s="20"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
     </row>
     <row r="5" ht="17" customHeight="1">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
+      <c r="A5" s="20"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
     </row>
     <row r="6" ht="17" customHeight="1">
-      <c r="A6" s="16"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
+      <c r="A6" s="20"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
     </row>
     <row r="7" ht="17" customHeight="1">
-      <c r="A7" s="16"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
+      <c r="A7" s="20"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
     </row>
     <row r="8" ht="17" customHeight="1">
-      <c r="A8" s="16"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
+      <c r="A8" s="20"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
     </row>
     <row r="9" ht="17" customHeight="1">
-      <c r="A9" s="16"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
+      <c r="A9" s="20"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
     </row>
     <row r="10" ht="17" customHeight="1">
-      <c r="A10" s="16"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
+      <c r="A10" s="20"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Few fields in TestData.excel updated.
</commit_message>
<xml_diff>
--- a/HybridFramework_Demo/src/test/resources/testData/TestData.xlsx
+++ b/HybridFramework_Demo/src/test/resources/testData/TestData.xlsx
@@ -1,19 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr checkCompatibility="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="2436" windowWidth="18264" windowHeight="5928"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId5"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -45,9 +49,6 @@
     <t>Home Price</t>
   </si>
   <si>
-    <t>Down Payment</t>
-  </si>
-  <si>
     <t>Mortgage Interest Rate</t>
   </si>
   <si>
@@ -96,31 +97,26 @@
     <t>07777777777</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="11"/>
-        <color indexed="11"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>tooolsqa@gmail.com</t>
-    </r>
-  </si>
-  <si>
     <t>Buy vs Rent</t>
   </si>
   <si>
     <t>22, LimeSquare, City Road</t>
+  </si>
+  <si>
+    <t>HomeLocation</t>
+  </si>
+  <si>
+    <t>DownPayment</t>
+  </si>
+  <si>
+    <t>Ben Claire, SD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -129,20 +125,10 @@
     <font>
       <sz val="12"/>
       <color indexed="8"/>
-      <name val="Helvetica"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
       <name val="Verdana"/>
     </font>
     <font>
-      <sz val="15"/>
-      <color indexed="8"/>
-      <name val="Verdana"/>
-    </font>
-    <font>
-      <b val="1"/>
+      <b/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
@@ -150,12 +136,6 @@
     <font>
       <sz val="11"/>
       <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="11"/>
-      <color indexed="11"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -348,78 +328,44 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="23">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="5" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -430,25 +376,82 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffdbe5f1"/>
-      <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ff0000ff"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFDBE5F1"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -640,7 +643,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -649,7 +652,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -658,7 +661,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -667,7 +670,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="40000" dist="20000" dir="5400000">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -676,7 +679,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="40000" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -685,7 +688,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="40000" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -797,8 +800,8 @@
     <a:spDef>
       <a:spPr>
         <a:blipFill rotWithShape="1">
-          <a:blip r:embed="rId1"/>
-          <a:srcRect l="0" t="0" r="0" b="0"/>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+          <a:srcRect/>
           <a:tile tx="0" ty="0" sx="100000" sy="100000" flip="none" algn="tl"/>
         </a:blipFill>
         <a:ln w="12700" cap="flat">
@@ -806,14 +809,14 @@
           <a:miter lim="400000"/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="50000"/>
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -832,7 +835,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1200" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -840,7 +843,7 @@
               <a:srgbClr val="FFFFFF"/>
             </a:solidFill>
             <a:effectLst>
-              <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="25400" dist="23998" dir="2700000">
+              <a:outerShdw blurRad="25400" dist="23998" dir="2700000" rotWithShape="0">
                 <a:srgbClr val="000000">
                   <a:alpha val="31034"/>
                 </a:srgbClr>
@@ -868,7 +871,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -894,7 +897,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -920,7 +923,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -946,7 +949,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -972,7 +975,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -998,7 +1001,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1024,7 +1027,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1050,7 +1053,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1076,7 +1079,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1089,9 +1092,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -1107,7 +1116,7 @@
         </a:ln>
         <a:effectLst/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1126,7 +1135,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1152,7 +1161,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1178,7 +1187,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1204,7 +1213,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1230,7 +1239,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1256,7 +1265,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1282,7 +1291,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1308,7 +1317,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1334,7 +1343,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1360,7 +1369,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1373,9 +1382,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1388,7 +1403,7 @@
         </a:ln>
         <a:effectLst/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1407,7 +1422,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1437,7 +1452,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1463,7 +1478,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1489,7 +1504,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1515,7 +1530,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1541,7 +1556,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1567,7 +1582,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1593,7 +1608,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1619,7 +1634,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1645,7 +1660,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1658,178 +1673,201 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:N11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IV11"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.625" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="6.61328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.25" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.25" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.75" style="1" customWidth="1"/>
-    <col min="5" max="5" width="7.875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="7.625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.25" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5" style="1" customWidth="1"/>
-    <col min="10" max="10" width="8.25" style="1" customWidth="1"/>
+    <col min="1" max="2" width="13.23046875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.3828125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.765625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="7.84375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="7.61328125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.4609375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.23046875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.4609375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="8.23046875" style="1" customWidth="1"/>
     <col min="11" max="11" width="15" style="1" customWidth="1"/>
-    <col min="12" max="12" width="15.25" style="1" customWidth="1"/>
-    <col min="13" max="13" width="16.875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="9.375" style="1" customWidth="1"/>
-    <col min="15" max="256" width="6.625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="15.23046875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="9.3828125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="11" style="22" customWidth="1"/>
+    <col min="15" max="15" width="10.23046875" style="22" customWidth="1"/>
+    <col min="16" max="16" width="8.15234375" style="22" customWidth="1"/>
+    <col min="17" max="17" width="8.15234375" style="1" customWidth="1"/>
+    <col min="18" max="256" width="6.61328125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="30" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="2">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="2">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="2">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s" s="2">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s" s="2">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s" s="2">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s" s="3">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s" s="3">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s" s="3">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s" s="3">
+      <c r="N1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+    </row>
+    <row r="2" spans="1:18" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" ht="17" customHeight="1">
-      <c r="A2" t="s" s="4">
+      <c r="B2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B2" t="s" s="4">
+      <c r="C2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C2" t="s" s="4">
+      <c r="D2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D2" t="s" s="4">
+      <c r="E2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E2" t="s" s="4">
+      <c r="F2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F2" t="s" s="4">
+      <c r="G2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G2" t="s" s="4">
+      <c r="H2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H2" t="s" s="4">
+      <c r="I2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I2" t="s" s="4">
+      <c r="J2" s="5"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="8"/>
+      <c r="R2" s="6"/>
+    </row>
+    <row r="3" spans="1:18" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="5"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="8"/>
-    </row>
-    <row r="3" ht="17" customHeight="1">
-      <c r="A3" t="s" s="4">
+      <c r="B3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B3" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s" s="4">
+      <c r="D3" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="D3" t="s" s="4">
-        <v>25</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
-      <c r="J3" t="s" s="4">
+      <c r="J3" s="4">
+        <v>80000</v>
+      </c>
+      <c r="K3" s="7">
+        <v>12</v>
+      </c>
+      <c r="L3" s="7"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="O3" s="4">
+        <v>20000</v>
+      </c>
+      <c r="R3" s="9"/>
+    </row>
+    <row r="4" spans="1:18" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="K3" t="s" s="9">
-        <v>27</v>
-      </c>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="8"/>
-    </row>
-    <row r="4" ht="17" customHeight="1">
-      <c r="A4" t="s" s="4">
-        <v>23</v>
-      </c>
-      <c r="B4" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s" s="4">
-        <v>28</v>
-      </c>
-      <c r="D4" t="s" s="4">
-        <v>25</v>
+      <c r="D4" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
-      <c r="G4" t="s" s="4">
-        <v>29</v>
+      <c r="G4" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
-      <c r="J4" t="s" s="4">
-        <v>26</v>
-      </c>
-      <c r="K4" s="6"/>
+      <c r="J4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" s="7"/>
       <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="8">
+      <c r="M4" s="8">
         <v>987879</v>
       </c>
-    </row>
-    <row r="5" ht="17" customHeight="1">
+      <c r="R4" s="6"/>
+    </row>
+    <row r="5" spans="1:18" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
@@ -1843,9 +1881,8 @@
       <c r="K5" s="12"/>
       <c r="L5" s="13"/>
       <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
-    </row>
-    <row r="6" ht="17" customHeight="1">
+    </row>
+    <row r="6" spans="1:18" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="15"/>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
@@ -1859,9 +1896,8 @@
       <c r="K6" s="12"/>
       <c r="L6" s="13"/>
       <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-    </row>
-    <row r="7" ht="17" customHeight="1">
+    </row>
+    <row r="7" spans="1:18" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="15"/>
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
@@ -1875,9 +1911,8 @@
       <c r="K7" s="12"/>
       <c r="L7" s="13"/>
       <c r="M7" s="14"/>
-      <c r="N7" s="14"/>
-    </row>
-    <row r="8" ht="17" customHeight="1">
+    </row>
+    <row r="8" spans="1:18" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="15"/>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
@@ -1891,9 +1926,8 @@
       <c r="K8" s="12"/>
       <c r="L8" s="13"/>
       <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-    </row>
-    <row r="9" ht="17" customHeight="1">
+    </row>
+    <row r="9" spans="1:18" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15"/>
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
@@ -1907,9 +1941,8 @@
       <c r="K9" s="12"/>
       <c r="L9" s="13"/>
       <c r="M9" s="14"/>
-      <c r="N9" s="14"/>
-    </row>
-    <row r="10" ht="17" customHeight="1">
+    </row>
+    <row r="10" spans="1:18" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="15"/>
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>
@@ -1923,9 +1956,8 @@
       <c r="K10" s="12"/>
       <c r="L10" s="13"/>
       <c r="M10" s="14"/>
-      <c r="N10" s="14"/>
-    </row>
-    <row r="11" ht="17" customHeight="1">
+    </row>
+    <row r="11" spans="1:18" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16"/>
       <c r="B11" s="17"/>
       <c r="C11" s="17"/>
@@ -1939,14 +1971,10 @@
       <c r="K11" s="17"/>
       <c r="L11" s="18"/>
       <c r="M11" s="19"/>
-      <c r="N11" s="19"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="K3" r:id="rId1" location="" tooltip="" display=""/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
   </headerFooter>
@@ -1954,85 +1982,80 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IV10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.625" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="6.61328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.625" style="20" customWidth="1"/>
-    <col min="2" max="2" width="6.625" style="20" customWidth="1"/>
-    <col min="3" max="3" width="6.625" style="20" customWidth="1"/>
-    <col min="4" max="4" width="6.625" style="20" customWidth="1"/>
-    <col min="5" max="5" width="6.625" style="20" customWidth="1"/>
-    <col min="6" max="256" width="6.625" style="20" customWidth="1"/>
+    <col min="1" max="256" width="6.61328125" style="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="17" customHeight="1">
+    <row r="1" spans="1:5" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="21"/>
       <c r="B1" s="21"/>
       <c r="C1" s="21"/>
       <c r="D1" s="21"/>
       <c r="E1" s="21"/>
     </row>
-    <row r="2" ht="17" customHeight="1">
+    <row r="2" spans="1:5" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="21"/>
       <c r="B2" s="21"/>
       <c r="C2" s="21"/>
       <c r="D2" s="21"/>
       <c r="E2" s="21"/>
     </row>
-    <row r="3" ht="17" customHeight="1">
+    <row r="3" spans="1:5" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="21"/>
       <c r="B3" s="21"/>
       <c r="C3" s="21"/>
       <c r="D3" s="21"/>
       <c r="E3" s="21"/>
     </row>
-    <row r="4" ht="17" customHeight="1">
+    <row r="4" spans="1:5" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="21"/>
       <c r="B4" s="21"/>
       <c r="C4" s="21"/>
       <c r="D4" s="21"/>
       <c r="E4" s="21"/>
     </row>
-    <row r="5" ht="17" customHeight="1">
+    <row r="5" spans="1:5" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="21"/>
       <c r="B5" s="21"/>
       <c r="C5" s="21"/>
       <c r="D5" s="21"/>
       <c r="E5" s="21"/>
     </row>
-    <row r="6" ht="17" customHeight="1">
+    <row r="6" spans="1:5" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="21"/>
       <c r="B6" s="21"/>
       <c r="C6" s="21"/>
       <c r="D6" s="21"/>
       <c r="E6" s="21"/>
     </row>
-    <row r="7" ht="17" customHeight="1">
+    <row r="7" spans="1:5" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="21"/>
       <c r="B7" s="21"/>
       <c r="C7" s="21"/>
       <c r="D7" s="21"/>
       <c r="E7" s="21"/>
     </row>
-    <row r="8" ht="17" customHeight="1">
+    <row r="8" spans="1:5" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="21"/>
       <c r="B8" s="21"/>
       <c r="C8" s="21"/>
       <c r="D8" s="21"/>
       <c r="E8" s="21"/>
     </row>
-    <row r="9" ht="17" customHeight="1">
+    <row r="9" spans="1:5" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="21"/>
       <c r="B9" s="21"/>
       <c r="C9" s="21"/>
       <c r="D9" s="21"/>
       <c r="E9" s="21"/>
     </row>
-    <row r="10" ht="17" customHeight="1">
+    <row r="10" spans="1:5" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="21"/>
       <c r="B10" s="21"/>
       <c r="C10" s="21"/>
@@ -2041,7 +2064,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="landscape" pageOrder="downThenOver"/>
+  <pageSetup orientation="landscape"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
   </headerFooter>
@@ -2049,85 +2072,80 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IV10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.625" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="6.61328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.625" style="22" customWidth="1"/>
-    <col min="2" max="2" width="6.625" style="22" customWidth="1"/>
-    <col min="3" max="3" width="6.625" style="22" customWidth="1"/>
-    <col min="4" max="4" width="6.625" style="22" customWidth="1"/>
-    <col min="5" max="5" width="6.625" style="22" customWidth="1"/>
-    <col min="6" max="256" width="6.625" style="22" customWidth="1"/>
+    <col min="1" max="256" width="6.61328125" style="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="17" customHeight="1">
+    <row r="1" spans="1:5" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="21"/>
       <c r="B1" s="21"/>
       <c r="C1" s="21"/>
       <c r="D1" s="21"/>
       <c r="E1" s="21"/>
     </row>
-    <row r="2" ht="17" customHeight="1">
+    <row r="2" spans="1:5" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="21"/>
       <c r="B2" s="21"/>
       <c r="C2" s="21"/>
       <c r="D2" s="21"/>
       <c r="E2" s="21"/>
     </row>
-    <row r="3" ht="17" customHeight="1">
+    <row r="3" spans="1:5" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="21"/>
       <c r="B3" s="21"/>
       <c r="C3" s="21"/>
       <c r="D3" s="21"/>
       <c r="E3" s="21"/>
     </row>
-    <row r="4" ht="17" customHeight="1">
+    <row r="4" spans="1:5" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="21"/>
       <c r="B4" s="21"/>
       <c r="C4" s="21"/>
       <c r="D4" s="21"/>
       <c r="E4" s="21"/>
     </row>
-    <row r="5" ht="17" customHeight="1">
+    <row r="5" spans="1:5" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="21"/>
       <c r="B5" s="21"/>
       <c r="C5" s="21"/>
       <c r="D5" s="21"/>
       <c r="E5" s="21"/>
     </row>
-    <row r="6" ht="17" customHeight="1">
+    <row r="6" spans="1:5" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="21"/>
       <c r="B6" s="21"/>
       <c r="C6" s="21"/>
       <c r="D6" s="21"/>
       <c r="E6" s="21"/>
     </row>
-    <row r="7" ht="17" customHeight="1">
+    <row r="7" spans="1:5" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="21"/>
       <c r="B7" s="21"/>
       <c r="C7" s="21"/>
       <c r="D7" s="21"/>
       <c r="E7" s="21"/>
     </row>
-    <row r="8" ht="17" customHeight="1">
+    <row r="8" spans="1:5" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="21"/>
       <c r="B8" s="21"/>
       <c r="C8" s="21"/>
       <c r="D8" s="21"/>
       <c r="E8" s="21"/>
     </row>
-    <row r="9" ht="17" customHeight="1">
+    <row r="9" spans="1:5" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="21"/>
       <c r="B9" s="21"/>
       <c r="C9" s="21"/>
       <c r="D9" s="21"/>
       <c r="E9" s="21"/>
     </row>
-    <row r="10" ht="17" customHeight="1">
+    <row r="10" spans="1:5" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="21"/>
       <c r="B10" s="21"/>
       <c r="C10" s="21"/>
@@ -2136,7 +2154,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="landscape" pageOrder="downThenOver"/>
+  <pageSetup orientation="landscape"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Updating the workspace.. Shubhankar
</commit_message>
<xml_diff>
--- a/HybridFramework_Demo/src/test/resources/testData/TestData.xlsx
+++ b/HybridFramework_Demo/src/test/resources/testData/TestData.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr checkCompatibility="1"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <bookViews>
-    <workbookView xWindow="0" yWindow="2436" windowWidth="18264" windowHeight="5928"/>
+    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="31">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -58,6 +52,12 @@
     <t>Monthly Rent</t>
   </si>
   <si>
+    <t>HomeLocation</t>
+  </si>
+  <si>
+    <t>DownPayment</t>
+  </si>
+  <si>
     <t>Framework_001</t>
   </si>
   <si>
@@ -94,29 +94,26 @@
     <t>Product 1</t>
   </si>
   <si>
+    <t>Ben Claire, SD</t>
+  </si>
+  <si>
+    <t>Buy vs Rent</t>
+  </si>
+  <si>
+    <t>22, LimeSquare, City Road</t>
+  </si>
+  <si>
     <t>07777777777</t>
-  </si>
-  <si>
-    <t>Buy vs Rent</t>
-  </si>
-  <si>
-    <t>22, LimeSquare, City Road</t>
-  </si>
-  <si>
-    <t>HomeLocation</t>
-  </si>
-  <si>
-    <t>DownPayment</t>
-  </si>
-  <si>
-    <t>Ben Claire, SD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="0" formatCode="General"/>
+  </numFmts>
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -125,10 +122,20 @@
     <font>
       <sz val="12"/>
       <color indexed="8"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
       <name val="Verdana"/>
     </font>
     <font>
-      <b/>
+      <sz val="15"/>
+      <color indexed="8"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <b val="1"/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
@@ -153,7 +160,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -216,6 +223,51 @@
         <color indexed="10"/>
       </left>
       <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
       <top style="thin">
         <color indexed="8"/>
       </top>
@@ -228,13 +280,6 @@
       <top style="thin">
         <color indexed="8"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -311,61 +356,104 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+  <cellXfs count="31">
+    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -376,82 +464,24 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFDBE5F1"/>
-      <rgbColor rgb="FFAAAAAA"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
+      <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffff0000"/>
+      <rgbColor rgb="ff00ff00"/>
+      <rgbColor rgb="ff0000ff"/>
+      <rgbColor rgb="ffffff00"/>
+      <rgbColor rgb="ffff00ff"/>
+      <rgbColor rgb="ff00ffff"/>
+      <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffdbe5f1"/>
+      <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -643,7 +673,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -652,7 +682,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -661,7 +691,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -670,7 +700,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="40000" dist="20000" dir="5400000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -679,7 +709,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="40000" dist="23000" dir="5400000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -688,7 +718,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="40000" dist="23000" dir="5400000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -800,8 +830,8 @@
     <a:spDef>
       <a:spPr>
         <a:blipFill rotWithShape="1">
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-          <a:srcRect/>
+          <a:blip r:embed="rId1"/>
+          <a:srcRect l="0" t="0" r="0" b="0"/>
           <a:tile tx="0" ty="0" sx="100000" sy="100000" flip="none" algn="tl"/>
         </a:blipFill>
         <a:ln w="12700" cap="flat">
@@ -809,14 +839,14 @@
           <a:miter lim="400000"/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
             <a:srgbClr val="000000">
               <a:alpha val="50000"/>
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -835,7 +865,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1200" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -843,7 +873,7 @@
               <a:srgbClr val="FFFFFF"/>
             </a:solidFill>
             <a:effectLst>
-              <a:outerShdw blurRad="25400" dist="23998" dir="2700000" rotWithShape="0">
+              <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="25400" dist="23998" dir="2700000">
                 <a:srgbClr val="000000">
                   <a:alpha val="31034"/>
                 </a:srgbClr>
@@ -871,7 +901,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -897,7 +927,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -923,7 +953,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -949,7 +979,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -975,7 +1005,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1001,7 +1031,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1027,7 +1057,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1053,7 +1083,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1079,7 +1109,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1092,15 +1122,9 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -1116,7 +1140,7 @@
         </a:ln>
         <a:effectLst/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1135,7 +1159,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1161,7 +1185,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1187,7 +1211,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1213,7 +1237,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1239,7 +1263,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1265,7 +1289,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1291,7 +1315,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1317,7 +1341,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1343,7 +1367,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1369,7 +1393,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1382,15 +1406,9 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1403,7 +1421,7 @@
         </a:ln>
         <a:effectLst/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1422,7 +1440,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1452,7 +1470,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1478,7 +1496,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1504,7 +1522,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1530,7 +1548,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1556,7 +1574,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1582,7 +1600,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1608,7 +1626,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1634,7 +1652,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1660,7 +1678,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1673,488 +1691,346 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IV11"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.61328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="6.625" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="2" width="13.23046875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.3828125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.765625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="7.84375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="7.61328125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="20.4609375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.23046875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.4609375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="8.23046875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.25" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.25" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.75" style="1" customWidth="1"/>
+    <col min="5" max="5" width="7.875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="7.625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.25" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5" style="1" customWidth="1"/>
+    <col min="10" max="10" width="8.25" style="1" customWidth="1"/>
     <col min="11" max="11" width="15" style="1" customWidth="1"/>
-    <col min="12" max="12" width="15.23046875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="9.3828125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="11" style="22" customWidth="1"/>
-    <col min="15" max="15" width="10.23046875" style="22" customWidth="1"/>
-    <col min="16" max="16" width="8.15234375" style="22" customWidth="1"/>
-    <col min="17" max="17" width="8.15234375" style="1" customWidth="1"/>
-    <col min="18" max="256" width="6.61328125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="15.25" style="1" customWidth="1"/>
+    <col min="13" max="13" width="9.375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="11" style="1" customWidth="1"/>
+    <col min="15" max="15" width="10.25" style="1" customWidth="1"/>
+    <col min="16" max="16" width="8.125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="8.125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="6.625" style="1" customWidth="1"/>
+    <col min="19" max="256" width="6.625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" ht="30" customHeight="1">
+      <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s" s="2">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s" s="2">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s" s="2">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" t="s" s="2">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" t="s" s="2">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" t="s" s="2">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" t="s" s="2">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" t="s" s="2">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" t="s" s="2">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" t="s" s="3">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" t="s" s="3">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" t="s" s="3">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
+      <c r="N1" t="s" s="3">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s" s="3">
+        <v>14</v>
+      </c>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
     </row>
-    <row r="2" spans="1:18" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="4" t="s">
+    <row r="2" ht="16.95" customHeight="1">
+      <c r="A2" t="s" s="5">
         <v>15</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="B2" t="s" s="5">
         <v>16</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="C2" t="s" s="5">
         <v>17</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="D2" t="s" s="5">
         <v>18</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="E2" t="s" s="5">
         <v>19</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="F2" t="s" s="5">
         <v>20</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="G2" t="s" s="5">
         <v>21</v>
       </c>
-      <c r="J2" s="5"/>
+      <c r="H2" t="s" s="5">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s" s="5">
+        <v>23</v>
+      </c>
+      <c r="J2" s="6"/>
       <c r="K2" s="7"/>
       <c r="L2" s="7"/>
       <c r="M2" s="8"/>
-      <c r="R2" s="6"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="12"/>
+      <c r="R2" s="7"/>
     </row>
-    <row r="3" spans="1:18" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="4" t="s">
+    <row r="3" ht="16.95" customHeight="1">
+      <c r="A3" t="s" s="5">
         <v>24</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="4">
+      <c r="B3" t="s" s="5">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s" s="5">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s" s="5">
+        <v>26</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="5">
         <v>80000</v>
       </c>
       <c r="K3" s="7">
         <v>12</v>
       </c>
       <c r="L3" s="7"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="4" t="s">
+      <c r="M3" s="7"/>
+      <c r="N3" t="s" s="5">
+        <v>27</v>
+      </c>
+      <c r="O3" s="5">
+        <v>20000</v>
+      </c>
+      <c r="P3" s="13"/>
+      <c r="Q3" s="12"/>
+      <c r="R3" s="7"/>
+    </row>
+    <row r="4" ht="16.95" customHeight="1">
+      <c r="A4" t="s" s="5">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s" s="5">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s" s="5">
+        <v>28</v>
+      </c>
+      <c r="D4" t="s" s="5">
+        <v>26</v>
+      </c>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" t="s" s="5">
+        <v>29</v>
+      </c>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" t="s" s="5">
         <v>30</v>
-      </c>
-      <c r="O3" s="4">
-        <v>20000</v>
-      </c>
-      <c r="R3" s="9"/>
-    </row>
-    <row r="4" spans="1:18" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="4" t="s">
-        <v>25</v>
       </c>
       <c r="K4" s="7"/>
       <c r="L4" s="7"/>
       <c r="M4" s="8">
         <v>987879</v>
       </c>
-      <c r="R4" s="6"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="12"/>
+      <c r="R4" s="7"/>
     </row>
-    <row r="5" spans="1:18" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="10"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="14"/>
+    <row r="5" ht="16.95" customHeight="1">
+      <c r="A5" s="16"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="22"/>
     </row>
-    <row r="6" spans="1:18" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="15"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="14"/>
+    <row r="6" ht="16.95" customHeight="1">
+      <c r="A6" s="23"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="21"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="22"/>
     </row>
-    <row r="7" spans="1:18" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="15"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="14"/>
+    <row r="7" ht="16.95" customHeight="1">
+      <c r="A7" s="23"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
+      <c r="R7" s="22"/>
     </row>
-    <row r="8" spans="1:18" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="15"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="14"/>
+    <row r="8" ht="16.95" customHeight="1">
+      <c r="A8" s="23"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="21"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11"/>
+      <c r="R8" s="22"/>
     </row>
-    <row r="9" spans="1:18" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="15"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="14"/>
+    <row r="9" ht="16.95" customHeight="1">
+      <c r="A9" s="23"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="21"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="22"/>
     </row>
-    <row r="10" spans="1:18" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="15"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="14"/>
+    <row r="10" ht="16.95" customHeight="1">
+      <c r="A10" s="23"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="21"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="22"/>
     </row>
-    <row r="11" spans="1:18" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="16"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="18"/>
-      <c r="M11" s="19"/>
+    <row r="11" ht="16.95" customHeight="1">
+      <c r="A11" s="24"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="26"/>
+      <c r="M11" s="27"/>
+      <c r="N11" s="28"/>
+      <c r="O11" s="29"/>
+      <c r="P11" s="29"/>
+      <c r="Q11" s="29"/>
+      <c r="R11" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait"/>
-  <headerFooter>
-    <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IV10"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="6.61328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="256" width="6.61328125" style="20" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="21"/>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-    </row>
-    <row r="2" spans="1:5" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-    </row>
-    <row r="3" spans="1:5" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="21"/>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-    </row>
-    <row r="4" spans="1:5" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="21"/>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-    </row>
-    <row r="5" spans="1:5" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="21"/>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-    </row>
-    <row r="6" spans="1:5" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="21"/>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-    </row>
-    <row r="7" spans="1:5" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="21"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-    </row>
-    <row r="8" spans="1:5" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="21"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-    </row>
-    <row r="9" spans="1:5" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="21"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-    </row>
-    <row r="10" spans="1:5" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="21"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="landscape"/>
-  <headerFooter>
-    <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IV10"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="6.61328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="256" width="6.61328125" style="22" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="21"/>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-    </row>
-    <row r="2" spans="1:5" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-    </row>
-    <row r="3" spans="1:5" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="21"/>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-    </row>
-    <row r="4" spans="1:5" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="21"/>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-    </row>
-    <row r="5" spans="1:5" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="21"/>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-    </row>
-    <row r="6" spans="1:5" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="21"/>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-    </row>
-    <row r="7" spans="1:5" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="21"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-    </row>
-    <row r="8" spans="1:5" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="21"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-    </row>
-    <row r="9" spans="1:5" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="21"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-    </row>
-    <row r="10" spans="1:5" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="21"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="landscape"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
   </headerFooter>

</xml_diff>